<commit_message>
- automatically create missing Excel files when using any of the `write*()` commands. - allow the reading of an empty cell range follow by other Excel operations such as `transpose()`. - [`clear(file,worksheet,range)`]: now clearing a non-existent file or worksheet would not throw any error.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/script/jmeter-showcase.xlsx
+++ b/src/test/resources/showcase/artifact/script/jmeter-showcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D769CD72-636C-3F43-9C2E-8069F076ADF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A25589E-877D-8B47-B6A0-3F3C2255CA29}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10960" windowWidth="51200" windowHeight="21040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="1220" windowWidth="34120" windowHeight="31560" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="xml">'#system'!$AA$2:$AA$11</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="632">
   <si>
     <t>description</t>
   </si>
@@ -1865,9 +1865,6 @@
     <t>[TEXT(${testname.var}) =&gt; text]</t>
   </si>
   <si>
-    <t>working on [XML(${target.location}) =&gt; store(newJmx) count(${testname.xpath_esc})] test names in ${target.location}</t>
-  </si>
-  <si>
     <t>[XML(newJmx) =&gt; text]</t>
   </si>
   <si>
@@ -1898,42 +1895,173 @@
     <t>Update variables</t>
   </si>
   <si>
-    <t>Updating testname ${testname}, enabled=[XML(newJmx) =&gt; 
+    <t>make sure new JMX file is removed</t>
+  </si>
+  <si>
+    <t>Search-n-Replace</t>
+  </si>
+  <si>
+    <t>search and replace based on config</t>
+  </si>
+  <si>
+    <t>searchAndReplace(file,config,saveAs)</t>
+  </si>
+  <si>
+    <t>${search/configFile}</t>
+  </si>
+  <si>
+    <t>${target.newLocation}2</t>
+  </si>
+  <si>
+    <t>${target.newLocation}3</t>
+  </si>
+  <si>
+    <t>list out all available variables</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>${variable.prefix}</t>
+  </si>
+  <si>
+    <t>[LIST(${variables}) =&gt; length]</t>
+  </si>
+  <si>
+    <r>
+      <t>Updating testname ${testname}, enabled=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>[XML(newJmx) =&gt; 
  updateAttribute(${xpath},enabled,${testname.enabled}) 
  store(newJmx) 
  extract(//*[@testname='${testname}']/@enabled)
 ]</t>
-  </si>
-  <si>
-    <t>make sure new JMX file is removed</t>
-  </si>
-  <si>
-    <t>write updated XML to output as savepoint, also sub variables with actual values</t>
-  </si>
-  <si>
-    <t>Search-n-Replace</t>
-  </si>
-  <si>
-    <t>search and replace based on config</t>
-  </si>
-  <si>
-    <t>searchAndReplace(file,config,saveAs)</t>
-  </si>
-  <si>
-    <t>${search/configFile}</t>
-  </si>
-  <si>
-    <t>${target.newLocation}2</t>
-  </si>
-  <si>
-    <t>${target.newLocation}3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">working on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>[XML(${target.location}) =&gt; store(newJmx) count(${testname.xpath_esc})]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> test names in ${target.location}</t>
+    </r>
+  </si>
+  <si>
+    <t>perform variable substitution on `jmxText`</t>
+  </si>
+  <si>
+    <t>[LIST(${variables}) =&gt; item(${index}) text append(}) prepend(${)]</t>
+  </si>
+  <si>
+    <t>variable.value</t>
+  </si>
+  <si>
+    <t>[TEXT(${variable.name}) =&gt; text]</t>
+  </si>
+  <si>
+    <t>variable.name</t>
+  </si>
+  <si>
+    <t>target variable</t>
+  </si>
+  <si>
+    <t>[LIST(${variables}) =&gt; item(${index}) text removeStart(${variable.prefix})]</t>
+  </si>
+  <si>
+    <t>LOOP: handle each found variable</t>
+  </si>
+  <si>
+    <t>Replacing ${jmeterVariableCount} variables in ${target.location}</t>
+  </si>
+  <si>
+    <t>- derive variable name</t>
+  </si>
+  <si>
+    <t>- derive variable value</t>
+  </si>
+  <si>
+    <t>- perform replacement</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>replace JMX file of length [XML(newJmx) =&gt; text store(jmxText) length].</t>
+  </si>
+  <si>
+    <t>[TEXT(jmxText) =&gt; text]</t>
+  </si>
+  <si>
+    <t>write updated XML to output as savepoint</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Replacing variables in JMX file of length </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>[TEXT(jmxText) =&gt; 
+ replaceRegex(\$\{${target variable}\},${variable.value}) 
+ text 
+ store(jmxText) 
+ length
+]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>go to next testname</t>
+  </si>
+  <si>
+    <t>go to next variable</t>
+  </si>
+  <si>
+    <t>- derive the variable to look for (without ${…})</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2013,6 +2141,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <family val="2"/>
     </font>
@@ -2106,7 +2241,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2268,6 +2403,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3489,7 +3644,7 @@
         <v>295</v>
       </c>
       <c r="J19" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="V19" t="s">
         <v>106</v>
@@ -4687,7 +4842,7 @@
         <v>479</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -21383,11 +21538,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42103101-CB63-AA4F-9710-638DEEF16C96}">
-  <dimension ref="A1:O1005"/>
+  <dimension ref="A1:O1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21396,7 +21551,7 @@
     <col min="2" max="2" width="45.5" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.83203125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="37.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="56.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="61.33203125" style="9" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="23.83203125" style="9" customWidth="1" collapsed="1"/>
     <col min="7" max="9" width="21" style="9" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="25.1640625" style="22" customWidth="1" collapsed="1"/>
@@ -21520,7 +21675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>468</v>
       </c>
@@ -21549,10 +21704,10 @@
       <c r="N5" s="14"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>14</v>
@@ -21561,9 +21716,11 @@
         <v>38</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>591</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>590</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>522</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -21574,7 +21731,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>572</v>
       </c>
@@ -21603,7 +21760,7 @@
       <c r="N7" s="14"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
       <c r="B8" s="4"/>
       <c r="C8" s="12" t="s">
@@ -21628,7 +21785,7 @@
       <c r="N8" s="14"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
       <c r="B9" s="4"/>
       <c r="C9" s="12" t="s">
@@ -21653,7 +21810,7 @@
       <c r="N9" s="14"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25"/>
       <c r="B10" s="4"/>
       <c r="C10" s="12" t="s">
@@ -21663,7 +21820,7 @@
         <v>69</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>589</v>
+        <v>611</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="6"/>
@@ -21676,10 +21833,10 @@
       <c r="N10" s="14"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="36" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>13</v>
@@ -21688,7 +21845,7 @@
         <v>320</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>578</v>
@@ -21703,7 +21860,7 @@
       <c r="N11" s="14"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="37"/>
       <c r="C12" s="12" t="s">
@@ -21728,10 +21885,10 @@
       <c r="N12" s="14"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="37" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>13</v>
@@ -21755,10 +21912,10 @@
       <c r="N13" s="14"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
       <c r="B14" s="37" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>13</v>
@@ -21782,10 +21939,10 @@
       <c r="N14" s="14"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
       <c r="B15" s="37" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>13</v>
@@ -21809,10 +21966,10 @@
       <c r="N15" s="14"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
       <c r="B16" s="37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>13</v>
@@ -21846,7 +22003,7 @@
         <v>69</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="6"/>
@@ -21859,9 +22016,11 @@
       <c r="N17" s="14"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25"/>
-      <c r="B18" s="37"/>
+      <c r="B18" s="37" t="s">
+        <v>629</v>
+      </c>
       <c r="C18" s="12" t="s">
         <v>51</v>
       </c>
@@ -21884,9 +22043,9 @@
       <c r="N18" s="14"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25"/>
-      <c r="B19" s="37"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="12" t="s">
         <v>14</v>
       </c>
@@ -21894,10 +22053,10 @@
         <v>433</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>522</v>
@@ -21911,28 +22070,26 @@
       <c r="N19" s="14"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>599</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>606</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>84</v>
+        <v>574</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>607</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>590</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>522</v>
-      </c>
+        <v>608</v>
+      </c>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="21"/>
@@ -21942,28 +22099,22 @@
       <c r="N20" s="14"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
-        <v>603</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>604</v>
-      </c>
+    <row r="21" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="46"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>605</v>
+        <v>62</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>607</v>
+        <v>493</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>606</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>608</v>
-      </c>
+        <v>609</v>
+      </c>
+      <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="21"/>
@@ -21973,13 +22124,21 @@
       <c r="N21" s="14"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+    <row r="22" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>579</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -21990,13 +22149,20 @@
       <c r="N22" s="14"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+    <row r="23" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="48" t="s">
+        <v>612</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>625</v>
+      </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -22007,12 +22173,18 @@
       <c r="N23" s="14"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+    <row r="24" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>620</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -22024,13 +22196,23 @@
       <c r="N24" s="14"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+    <row r="25" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="46"/>
+      <c r="B25" s="49" t="s">
+        <v>619</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>578</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -22041,13 +22223,21 @@
       <c r="N25" s="14"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+    <row r="26" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>499</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -22058,13 +22248,23 @@
       <c r="N26" s="14"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="25"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+    <row r="27" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="46"/>
+      <c r="B27" s="50" t="s">
+        <v>621</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>613</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -22075,13 +22275,23 @@
       <c r="N27" s="14"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+    <row r="28" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="46"/>
+      <c r="B28" s="50" t="s">
+        <v>622</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>615</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -22092,13 +22302,23 @@
       <c r="N28" s="14"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+    <row r="29" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="46"/>
+      <c r="B29" s="50" t="s">
+        <v>631</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>618</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -22109,13 +22329,20 @@
       <c r="N29" s="14"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+    <row r="30" spans="1:15" ht="112" x14ac:dyDescent="0.2">
+      <c r="A30" s="46"/>
+      <c r="B30" s="50" t="s">
+        <v>623</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>628</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -22126,13 +22353,23 @@
       <c r="N30" s="14"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="6"/>
+    <row r="31" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="46"/>
+      <c r="B31" s="50" t="s">
+        <v>630</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>505</v>
+      </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -22143,14 +22380,26 @@
       <c r="N31" s="14"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+    <row r="32" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>522</v>
+      </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="21"/>
@@ -22160,14 +22409,28 @@
       <c r="N32" s="14"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+    <row r="33" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>605</v>
+      </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="21"/>
@@ -22177,7 +22440,7 @@
       <c r="N33" s="14"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25"/>
       <c r="B34" s="4"/>
       <c r="C34" s="12"/>
@@ -22194,7 +22457,7 @@
       <c r="N34" s="14"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25"/>
       <c r="B35" s="4"/>
       <c r="C35" s="12"/>
@@ -22211,7 +22474,7 @@
       <c r="N35" s="14"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25"/>
       <c r="B36" s="4"/>
       <c r="C36" s="12"/>
@@ -22335,7 +22598,7 @@
       <c r="B43" s="4"/>
       <c r="C43" s="12"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -22366,7 +22629,7 @@
     </row>
     <row r="45" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25"/>
-      <c r="B45" s="4"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="12"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -32717,25 +32980,217 @@
       <c r="N653" s="14"/>
       <c r="O653" s="2"/>
     </row>
-    <row r="654" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A654" s="25"/>
+      <c r="B654" s="4"/>
+      <c r="C654" s="12"/>
+      <c r="D654" s="6"/>
+      <c r="E654" s="6"/>
+      <c r="F654" s="6"/>
+      <c r="G654" s="6"/>
+      <c r="H654" s="6"/>
+      <c r="I654" s="6"/>
+      <c r="J654" s="21"/>
+      <c r="K654" s="2"/>
+      <c r="L654" s="14"/>
+      <c r="M654" s="11"/>
+      <c r="N654" s="14"/>
+      <c r="O654" s="2"/>
+    </row>
+    <row r="655" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A655" s="25"/>
+      <c r="B655" s="4"/>
+      <c r="C655" s="12"/>
+      <c r="D655" s="6"/>
+      <c r="E655" s="6"/>
+      <c r="F655" s="6"/>
+      <c r="G655" s="6"/>
+      <c r="H655" s="6"/>
+      <c r="I655" s="6"/>
+      <c r="J655" s="21"/>
+      <c r="K655" s="2"/>
+      <c r="L655" s="14"/>
+      <c r="M655" s="11"/>
+      <c r="N655" s="14"/>
+      <c r="O655" s="2"/>
+    </row>
+    <row r="656" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A656" s="25"/>
+      <c r="B656" s="4"/>
+      <c r="C656" s="12"/>
+      <c r="D656" s="6"/>
+      <c r="E656" s="6"/>
+      <c r="F656" s="6"/>
+      <c r="G656" s="6"/>
+      <c r="H656" s="6"/>
+      <c r="I656" s="6"/>
+      <c r="J656" s="21"/>
+      <c r="K656" s="2"/>
+      <c r="L656" s="14"/>
+      <c r="M656" s="11"/>
+      <c r="N656" s="14"/>
+      <c r="O656" s="2"/>
+    </row>
+    <row r="657" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A657" s="25"/>
+      <c r="B657" s="4"/>
+      <c r="C657" s="12"/>
+      <c r="D657" s="6"/>
+      <c r="E657" s="6"/>
+      <c r="F657" s="6"/>
+      <c r="G657" s="6"/>
+      <c r="H657" s="6"/>
+      <c r="I657" s="6"/>
+      <c r="J657" s="21"/>
+      <c r="K657" s="2"/>
+      <c r="L657" s="14"/>
+      <c r="M657" s="11"/>
+      <c r="N657" s="14"/>
+      <c r="O657" s="2"/>
+    </row>
+    <row r="658" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A658" s="25"/>
+      <c r="B658" s="4"/>
+      <c r="C658" s="12"/>
+      <c r="D658" s="6"/>
+      <c r="E658" s="6"/>
+      <c r="F658" s="6"/>
+      <c r="G658" s="6"/>
+      <c r="H658" s="6"/>
+      <c r="I658" s="6"/>
+      <c r="J658" s="21"/>
+      <c r="K658" s="2"/>
+      <c r="L658" s="14"/>
+      <c r="M658" s="11"/>
+      <c r="N658" s="14"/>
+      <c r="O658" s="2"/>
+    </row>
+    <row r="659" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A659" s="25"/>
+      <c r="B659" s="4"/>
+      <c r="C659" s="12"/>
+      <c r="D659" s="6"/>
+      <c r="E659" s="6"/>
+      <c r="F659" s="6"/>
+      <c r="G659" s="6"/>
+      <c r="H659" s="6"/>
+      <c r="I659" s="6"/>
+      <c r="J659" s="21"/>
+      <c r="K659" s="2"/>
+      <c r="L659" s="14"/>
+      <c r="M659" s="11"/>
+      <c r="N659" s="14"/>
+      <c r="O659" s="2"/>
+    </row>
+    <row r="660" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A660" s="25"/>
+      <c r="B660" s="4"/>
+      <c r="C660" s="12"/>
+      <c r="D660" s="6"/>
+      <c r="E660" s="6"/>
+      <c r="F660" s="6"/>
+      <c r="G660" s="6"/>
+      <c r="H660" s="6"/>
+      <c r="I660" s="6"/>
+      <c r="J660" s="21"/>
+      <c r="K660" s="2"/>
+      <c r="L660" s="14"/>
+      <c r="M660" s="11"/>
+      <c r="N660" s="14"/>
+      <c r="O660" s="2"/>
+    </row>
+    <row r="661" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A661" s="25"/>
+      <c r="B661" s="4"/>
+      <c r="C661" s="12"/>
+      <c r="D661" s="6"/>
+      <c r="E661" s="6"/>
+      <c r="F661" s="6"/>
+      <c r="G661" s="6"/>
+      <c r="H661" s="6"/>
+      <c r="I661" s="6"/>
+      <c r="J661" s="21"/>
+      <c r="K661" s="2"/>
+      <c r="L661" s="14"/>
+      <c r="M661" s="11"/>
+      <c r="N661" s="14"/>
+      <c r="O661" s="2"/>
+    </row>
+    <row r="662" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A662" s="25"/>
+      <c r="B662" s="4"/>
+      <c r="C662" s="12"/>
+      <c r="D662" s="6"/>
+      <c r="E662" s="6"/>
+      <c r="F662" s="6"/>
+      <c r="G662" s="6"/>
+      <c r="H662" s="6"/>
+      <c r="I662" s="6"/>
+      <c r="J662" s="21"/>
+      <c r="K662" s="2"/>
+      <c r="L662" s="14"/>
+      <c r="M662" s="11"/>
+      <c r="N662" s="14"/>
+      <c r="O662" s="2"/>
+    </row>
+    <row r="663" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A663" s="25"/>
+      <c r="B663" s="4"/>
+      <c r="C663" s="12"/>
+      <c r="D663" s="6"/>
+      <c r="E663" s="6"/>
+      <c r="F663" s="6"/>
+      <c r="G663" s="6"/>
+      <c r="H663" s="6"/>
+      <c r="I663" s="6"/>
+      <c r="J663" s="21"/>
+      <c r="K663" s="2"/>
+      <c r="L663" s="14"/>
+      <c r="M663" s="11"/>
+      <c r="N663" s="14"/>
+      <c r="O663" s="2"/>
+    </row>
+    <row r="664" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A664" s="25"/>
+      <c r="B664" s="4"/>
+      <c r="C664" s="12"/>
+      <c r="D664" s="6"/>
+      <c r="E664" s="6"/>
+      <c r="F664" s="6"/>
+      <c r="G664" s="6"/>
+      <c r="H664" s="6"/>
+      <c r="I664" s="6"/>
+      <c r="J664" s="21"/>
+      <c r="K664" s="2"/>
+      <c r="L664" s="14"/>
+      <c r="M664" s="11"/>
+      <c r="N664" s="14"/>
+      <c r="O664" s="2"/>
+    </row>
+    <row r="665" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A665" s="25"/>
+      <c r="B665" s="4"/>
+      <c r="C665" s="12"/>
+      <c r="D665" s="6"/>
+      <c r="E665" s="6"/>
+      <c r="F665" s="6"/>
+      <c r="G665" s="6"/>
+      <c r="H665" s="6"/>
+      <c r="I665" s="6"/>
+      <c r="J665" s="21"/>
+      <c r="K665" s="2"/>
+      <c r="L665" s="14"/>
+      <c r="M665" s="11"/>
+      <c r="N665" s="14"/>
+      <c r="O665" s="2"/>
+    </row>
+    <row r="666" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" spans="1:15" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="673" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="674" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="675" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -33069,6 +33524,18 @@
     <row r="1003" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -33089,10 +33556,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C705" xr:uid="{E693959E-FB73-FD4A-AEA2-E7D4F18895ED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C717" xr:uid="{E693959E-FB73-FD4A-AEA2-E7D4F18895ED}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D703" xr:uid="{048E70AF-FC6A-AA4A-92FC-E2E25B50C744}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D715" xr:uid="{048E70AF-FC6A-AA4A-92FC-E2E25B50C744}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>